<commit_message>
Registro de actividades hasta 01_02
</commit_message>
<xml_diff>
--- a/data_act/base_actividades.xlsx
+++ b/data_act/base_actividades.xlsx
@@ -5,22 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Desktop\Curso_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\curso_python_poli_dec\data_act\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37C5D59E-7C8C-469A-8CFF-7B7A8E05FEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B46C808-141E-40FE-85BC-61E9CA9B1677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respuestas de formulario 1'!$B$1:$F$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Número de cédula</t>
   </si>
@@ -145,9 +161,6 @@
     <t>Correo</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad2 </t>
-  </si>
-  <si>
     <t>laura.castaneda@epn.edu.ec</t>
   </si>
   <si>
@@ -236,13 +249,28 @@
   </si>
   <si>
     <t>jhosueact@gmail.com</t>
+  </si>
+  <si>
+    <t>Python1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python2 </t>
+  </si>
+  <si>
+    <t>Python3</t>
+  </si>
+  <si>
+    <t>Actividad2</t>
+  </si>
+  <si>
+    <t>Python4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -267,6 +295,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -518,22 +552,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
     <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" customWidth="1"/>
-    <col min="5" max="9" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
+    <col min="6" max="9" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
@@ -544,10 +578,22 @@
         <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -557,8 +603,14 @@
       <c r="C2" s="1">
         <v>1752903938</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -569,13 +621,22 @@
         <v>1752651305</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -586,13 +647,22 @@
         <v>1759428368</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -603,13 +673,22 @@
         <v>1722073390</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -620,10 +699,16 @@
         <v>1750770503</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -634,13 +719,16 @@
         <v>1725116386</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -651,13 +739,16 @@
         <v>1004567580</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -668,13 +759,16 @@
         <v>1725838476</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -685,13 +779,25 @@
         <v>1751577238</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -702,13 +808,22 @@
         <v>1719620484</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -719,13 +834,19 @@
         <v>1726411364</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -736,13 +857,22 @@
         <v>1754088282</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -753,13 +883,25 @@
         <v>1754679312</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -770,13 +912,19 @@
         <v>1721341244</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -786,8 +934,11 @@
       <c r="C16" s="1">
         <v>1754346102</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -797,8 +948,20 @@
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -809,13 +972,13 @@
         <v>1719795070</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -826,13 +989,25 @@
         <v>1725264137</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -843,13 +1018,25 @@
         <v>1720331329</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -860,13 +1047,25 @@
         <v>1722746185</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -877,13 +1076,25 @@
         <v>1724175490</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -894,13 +1105,16 @@
         <v>1003771522</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -911,13 +1125,22 @@
         <v>1104290406</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -928,13 +1151,25 @@
         <v>1754573069</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -945,13 +1180,19 @@
         <v>1727170753</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -962,13 +1203,22 @@
         <v>7</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -979,13 +1229,25 @@
         <v>1751537687</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -996,10 +1258,22 @@
         <v>1754480398</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1010,13 +1284,22 @@
         <v>1753933058</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1027,13 +1310,22 @@
         <v>13</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1043,8 +1335,14 @@
       <c r="C32" s="1">
         <v>1719991216</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1055,13 +1353,19 @@
         <v>1500972763</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1072,13 +1376,25 @@
         <v>1752761419</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1089,13 +1405,16 @@
         <v>1754515185</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1110,6 +1429,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
     <sortCondition ref="B2:B36"/>
   </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D12" r:id="rId1" xr:uid="{E5CD8F21-D7D8-46B9-BCC1-3393BF9BA497}"/>
     <hyperlink ref="D31" r:id="rId2" xr:uid="{1875038E-EA37-4466-8F60-684C8FB42D7C}"/>

</xml_diff>

<commit_message>
Nueva base de datos con notas finales y documento que detalla el prroceso
</commit_message>
<xml_diff>
--- a/data_act/base_actividades.xlsx
+++ b/data_act/base_actividades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\curso_python_poli_dec\data_act\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B46C808-141E-40FE-85BC-61E9CA9B1677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABC6CED-AC4F-428F-8AEC-7E2985560988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
-  <si>
-    <t>Número de cédula</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Lema Narváez Karen Estefanía</t>
   </si>
@@ -59,27 +56,18 @@
     <t xml:space="preserve">Pilco Serrano Maritza Noemí </t>
   </si>
   <si>
-    <t>0605213529</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erazo Rodríguez Jéssica Lizbeth </t>
   </si>
   <si>
     <t>Mayo López Paula Samira</t>
   </si>
   <si>
-    <t>0504423781</t>
-  </si>
-  <si>
     <t xml:space="preserve">Salazar Torres Fernanda </t>
   </si>
   <si>
     <t xml:space="preserve">Salazar Chiliquinga Kerly Lisbeth </t>
   </si>
   <si>
-    <t>0504040908</t>
-  </si>
-  <si>
     <t>Cuichán Tacuri Jhosue Ariel</t>
   </si>
   <si>
@@ -254,16 +242,31 @@
     <t>Python1</t>
   </si>
   <si>
-    <t xml:space="preserve">Python2 </t>
-  </si>
-  <si>
     <t>Python3</t>
   </si>
   <si>
-    <t>Actividad2</t>
-  </si>
-  <si>
     <t>Python4</t>
+  </si>
+  <si>
+    <t>Python5</t>
+  </si>
+  <si>
+    <t>Dias1</t>
+  </si>
+  <si>
+    <t>Dias2</t>
+  </si>
+  <si>
+    <t>Dias3</t>
+  </si>
+  <si>
+    <t>Dias4</t>
+  </si>
+  <si>
+    <t>Python2</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -327,10 +330,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -552,237 +554,384 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" customWidth="1"/>
-    <col min="6" max="9" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1752903938</v>
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1752651305</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>68</v>
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1759428368</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1722073390</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>58</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>1</v>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1750770503</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>70</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1725116386</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>62</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1004567580</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>15</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1725838476</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1751577238</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -793,126 +942,183 @@
       <c r="H10">
         <v>1</v>
       </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
       <c r="J10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1719620484</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>60</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1726411364</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1754088282</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
       <c r="H13">
         <v>1</v>
       </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
       <c r="J13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1754679312</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
       <c r="J14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1721341244</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -920,267 +1126,411 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
       <c r="J15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1754346102</v>
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1719795070</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1725264137</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
-      <c r="G19">
-        <v>1</v>
+      <c r="G19" s="2">
+        <v>2</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
       <c r="J19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1720331329</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
       <c r="J20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1722746185</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
       <c r="J21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1724175490</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>66</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
       <c r="J22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1003771522</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>15</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1104290406</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>54</v>
+        <v>29</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>12</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1754573069</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>67</v>
+        <v>12</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
       <c r="J25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1727170753</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>64</v>
+        <v>18</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1188,22 +1538,37 @@
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
       <c r="J26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>15</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1214,22 +1579,34 @@
       <c r="G27">
         <v>1</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
       <c r="J27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>12</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1751537687</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1243,97 +1620,142 @@
       <c r="H28">
         <v>1</v>
       </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
       <c r="J28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1754480398</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>69</v>
+        <v>33</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
       <c r="H29">
         <v>1</v>
       </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
       <c r="J29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1753933058</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>12</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
       <c r="H31">
         <v>1</v>
       </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
       <c r="J31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1719991216</v>
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1341,45 +1763,78 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1500972763</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
       <c r="J33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>12</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1752761419</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1390,55 +1845,106 @@
       <c r="H34">
         <v>1</v>
       </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
       <c r="J34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1754515185</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" s="3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2">
+        <v>5</v>
       </c>
       <c r="J35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1752826220</v>
+        <v>32</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B36">
     <sortCondition ref="B2:B36"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" xr:uid="{E5CD8F21-D7D8-46B9-BCC1-3393BF9BA497}"/>
-    <hyperlink ref="D31" r:id="rId2" xr:uid="{1875038E-EA37-4466-8F60-684C8FB42D7C}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{A0CD7B77-6276-4805-A70B-4D8C77B0F76B}"/>
-    <hyperlink ref="D19" r:id="rId4" xr:uid="{EE9B0C77-0ABF-4958-957B-E7E14B8C495B}"/>
-    <hyperlink ref="D11" r:id="rId5" xr:uid="{3D29BB0D-2A82-461B-BFAC-53D7B962F3D1}"/>
-    <hyperlink ref="D18" r:id="rId6" xr:uid="{C8DBCB60-2736-4B05-A045-17340E3EEB66}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{8C7DE8EC-DE12-4CAE-AA04-9BCCD98ED141}"/>
-    <hyperlink ref="D29" r:id="rId8" xr:uid="{195724C2-02D1-4E7D-81C6-C95881253623}"/>
+    <hyperlink ref="C12" r:id="rId1" xr:uid="{E5CD8F21-D7D8-46B9-BCC1-3393BF9BA497}"/>
+    <hyperlink ref="C31" r:id="rId2" xr:uid="{1875038E-EA37-4466-8F60-684C8FB42D7C}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{A0CD7B77-6276-4805-A70B-4D8C77B0F76B}"/>
+    <hyperlink ref="C19" r:id="rId4" xr:uid="{EE9B0C77-0ABF-4958-957B-E7E14B8C495B}"/>
+    <hyperlink ref="C11" r:id="rId5" xr:uid="{3D29BB0D-2A82-461B-BFAC-53D7B962F3D1}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{C8DBCB60-2736-4B05-A045-17340E3EEB66}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{8C7DE8EC-DE12-4CAE-AA04-9BCCD98ED141}"/>
+    <hyperlink ref="C29" r:id="rId8" xr:uid="{195724C2-02D1-4E7D-81C6-C95881253623}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Datos en las bases
</commit_message>
<xml_diff>
--- a/data_act/base_actividades.xlsx
+++ b/data_act/base_actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\curso_python_poli_dec\data_act\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABC6CED-AC4F-428F-8AEC-7E2985560988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6F5AED-41DC-447B-9B65-DE52D5DB50E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Lema Narváez Karen Estefanía</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Ana Salet Hidalgo Flores</t>
+  </si>
+  <si>
+    <t>anitasalet2203@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -326,19 +332,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{9D73CA93-C885-46E9-B505-E72B375F0CA4}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -554,11 +564,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1817,7 +1827,7 @@
         <v>12</v>
       </c>
       <c r="L33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1928,6 +1938,44 @@
         <v>0</v>
       </c>
       <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>8</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+      <c r="I37" s="2">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
guia calificaciones y bases
</commit_message>
<xml_diff>
--- a/data_act/base_actividades.xlsx
+++ b/data_act/base_actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\curso_python_poli_dec\data_act\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6F5AED-41DC-447B-9B65-DE52D5DB50E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284CF4DA-6E46-46DC-A3D2-B01D9B3D26A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="348" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -337,12 +337,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
@@ -567,8 +566,8 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -586,7 +585,7 @@
     <col min="12" max="12" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
@@ -626,7 +625,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -658,10 +657,11 @@
         <v>12</v>
       </c>
       <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <f ca="1">RANDBETWEEN(0,10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -696,10 +696,11 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L3:L18" ca="1" si="0">RANDBETWEEN(0,10)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -734,10 +735,11 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -772,10 +774,11 @@
         <v>12</v>
       </c>
       <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -810,10 +813,11 @@
         <v>8</v>
       </c>
       <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,10 +852,11 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -886,10 +891,11 @@
         <v>15</v>
       </c>
       <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -924,10 +930,11 @@
         <v>8</v>
       </c>
       <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -962,10 +969,11 @@
         <v>2</v>
       </c>
       <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1000,10 +1008,11 @@
         <v>2</v>
       </c>
       <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1038,10 +1047,11 @@
         <v>2</v>
       </c>
       <c r="L12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1076,10 +1086,11 @@
         <v>2</v>
       </c>
       <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1114,10 +1125,11 @@
         <v>2</v>
       </c>
       <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1152,10 +1164,11 @@
         <v>12</v>
       </c>
       <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1187,10 +1200,11 @@
         <v>2</v>
       </c>
       <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1222,10 +1236,11 @@
         <v>2</v>
       </c>
       <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1260,10 +1275,11 @@
         <v>2</v>
       </c>
       <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1298,10 +1314,11 @@
         <v>2</v>
       </c>
       <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L18:L37" ca="1" si="1">RANDBETWEEN(0,10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1336,10 +1353,11 @@
         <v>2</v>
       </c>
       <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1374,10 +1392,11 @@
         <v>2</v>
       </c>
       <c r="L21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1412,10 +1431,11 @@
         <v>2</v>
       </c>
       <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1450,10 +1470,11 @@
         <v>15</v>
       </c>
       <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1488,10 +1509,11 @@
         <v>12</v>
       </c>
       <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1526,10 +1548,11 @@
         <v>2</v>
       </c>
       <c r="L25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1564,10 +1587,11 @@
         <v>15</v>
       </c>
       <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1602,10 +1626,11 @@
         <v>12</v>
       </c>
       <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1640,10 +1665,11 @@
         <v>2</v>
       </c>
       <c r="L28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1678,10 +1704,11 @@
         <v>2</v>
       </c>
       <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1716,10 +1743,11 @@
         <v>12</v>
       </c>
       <c r="L30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1754,10 +1782,11 @@
         <v>2</v>
       </c>
       <c r="L31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1789,10 +1818,11 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1827,10 +1857,11 @@
         <v>12</v>
       </c>
       <c r="L33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1865,10 +1896,11 @@
         <v>2</v>
       </c>
       <c r="L34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1903,10 +1935,11 @@
         <v>0</v>
       </c>
       <c r="L35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1938,7 +1971,8 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1948,7 +1982,7 @@
       <c r="B37" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D37">
@@ -1976,6 +2010,7 @@
         <v>0</v>
       </c>
       <c r="L37">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>